<commit_message>
Base de dados de Talentos pronta
</commit_message>
<xml_diff>
--- a/data/talentos.xlsx
+++ b/data/talentos.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="talentos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,32 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="315">
   <si>
     <t>ALIADOS QUIETOS</t>
   </si>
   <si>
-    <t>nome</t>
-  </si>
-  <si>
-    <t>nivel</t>
-  </si>
-  <si>
-    <t>pre-requisito</t>
-  </si>
-  <si>
     <t>especialista em Furtividade</t>
   </si>
   <si>
-    <t>descricao</t>
-  </si>
-  <si>
     <t>Você é habilidoso em se mover com um grupo. Quando estiver Evitando Ser Percebido e seus aliados Seguirem o Especialista, você e esses aliados podem rolar um único teste de Furtividade, usando o menor modificador, em vez de rolar separadamente. Isto não se aplica a rolagens de iniciativa.</t>
   </si>
   <si>
-    <t>tipos</t>
-  </si>
-  <si>
     <t>GERAL</t>
   </si>
   <si>
@@ -80,9 +65,6 @@
     <t>Você possui talento excepcional com um tipo de performance. Você recebe +1 de bônus de circunstância quando realizar um determinado tipo de performance. Se for mestre em Performance, este bônus aumenta para +2. Selecione uma das especialidades a seguir e aplique o bônus quando realizar testes de Performance desse tipo. Se não for claro quando uma especialidade se aplica, o MJ decide.</t>
   </si>
   <si>
-    <t>acao</t>
-  </si>
-  <si>
     <t>ASSUSTAR ATÉ A MORTE</t>
   </si>
   <si>
@@ -173,9 +155,6 @@
     <t>COAGIR GRUPO</t>
   </si>
   <si>
-    <t>treinado em Intimidaçã</t>
-  </si>
-  <si>
     <t>Quando Coagir, você pode comparar o resultado de seu teste deIntimidação às CDs de Vontade de dois alvos em vez de um. É possívelobter um grau de sucesso diferente para cada alvo. A quantidade dealvos que você pode Coagir em uma única ação aumenta para quatrose for especialista, 10 se for mestre e 25 se for lendário.</t>
   </si>
   <si>
@@ -609,6 +588,387 @@
   </si>
   <si>
     <t>CURA</t>
+  </si>
+  <si>
+    <t>MEDICINA NATURAL</t>
+  </si>
+  <si>
+    <t>treinado em Natureza</t>
+  </si>
+  <si>
+    <t>Você pode aplicar curas naturais para curar seus aliados. Você pode utilizar Natureza em vez de Medicina para Tratar Ferimentos. Se estiver em terras ermas, você pode ter acesso mais fácil a ingredientes frescos, permitindo que receba +2 de bônus de circunstância em seu teste para Tratar Ferimentos utilizando Natureza, sujeito ao arbítrio do MJ.</t>
+  </si>
+  <si>
+    <t>MÉDICO DE ENFERMARIA</t>
+  </si>
+  <si>
+    <t>especialista em Medicina</t>
+  </si>
+  <si>
+    <t>Você estudou em grandes enfermarias médicas, tratando vários pacientes de uma vez e cuidando de todas suas necessidades. Quando usar Tratar Doença ou Tratar Ferimentos, você pode tratar até dois alvos. Se for mestre em Medicina, você pode tratar até quatro alvos e, se for lendário em Medicina, pode tratar até oito alvos.</t>
+  </si>
+  <si>
+    <t>MÉDICO LENDÁRIO</t>
+  </si>
+  <si>
+    <t>lendário em Medicina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você descobriu avanços ou técnicas médicas que alcançam resultados milagrosos. Uma vez por dia para cada alvo, você pode gastar 1 hora tratando o alvo e fazer um teste de Medicina para remover uma doença ou a condição cego, condenado, drenado ou surdo. Utilize a CD da doença ou da magia ou efeito que criou a condição. Se a fonte do efeito for um artefato, acima de 20º nível ou similarmente poderosa, aumente a CD em 10. </t>
+  </si>
+  <si>
+    <t>MENTE NA MINHA CARA</t>
+  </si>
+  <si>
+    <t>Você pode utilizar Dissimulação para armar armadilhas para pegar qualquer um tentando lhe enganar. Se puder engajar em conversa com alguém tentando Mentir para você, utilize sua CD de Dissimulação se ela for maior que sua CD de Percepção para determinar se esse alguém obtém sucesso. Isto não se aplica se você não for capaz de dialogar contra-argumentando, como quando alguém tenta Mentir durante um discurso longo.</t>
+  </si>
+  <si>
+    <t>MENTIROSO CHARMOSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seu charme permite persuadir aqueles para quem você mente. Quando obtiver um sucesso crítico usando a ação Mentir, a atitude do alvo em relação a você melhora em um passo, como se você tivesse obtido sucesso em Diplomacia para Impressionar. Isto funciona somente uma vez por conversa, e se você tiver obtido um sucesso crítico contra vários alvos usando o mesmo resultado, escolha a atitude de uma criatura para aprimorar. Você deve estar mentindo para contar uma informação aparentemente importante, inflar sua condição ou se dar as boas graças, o que mentiras triviais e irrelevantes não conseguem alcançar. </t>
+  </si>
+  <si>
+    <t>NATAÇÃO RÁPIDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quando Nadar, você se move 1,5 metros a mais em um sucesso e 3 metros a mais em um sucesso crítico, até o máximo de sua Velocidade. Se for lendário em Atletismo, você recebe uma Velocidade de natação igual à sua Velocidade. </t>
+  </si>
+  <si>
+    <t>NEGOCIAÇÃO LENDÁRIA</t>
+  </si>
+  <si>
+    <t>lendário em Diplomacia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você pode negociar incrivelmente rápido em situações adversas. Você pode tentar Impressionar e então Pedir que seu oponente pare a atividade atual dele e engaje em negociações. Você sofre –5 de penalidade em seu teste de Diplomacia. O MJ determina a CD do Pedido baseado nas circunstâncias — isso normalmente possui uma CD pelo menos muito difícil do nível da criatura. Algumas criaturas podem simplesmente recusar, e mesmo criaturas que concordarem em negociar podem achar seus argumentos infundados e retornar à violência. </t>
+  </si>
+  <si>
+    <t>OLHAR INTIMIDANTE</t>
+  </si>
+  <si>
+    <t>Você pode Desmoralizar com um mero olhar. Quando o fizer, Desmoralizar perde o traço auditivo e adquire o traço visual, e você não sofre uma penalidade se a criatura não compreender seu idioma.</t>
+  </si>
+  <si>
+    <t>ORIENTAÇÃO DIVINA</t>
+  </si>
+  <si>
+    <t>lendário em Religião</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você é tão imerso em escrituras divinas que encontra significado e orientação em seus textos em qualquer situação. Gaste 10 minutos Decifrando Escrita em escrituras religiosas de sua divindade ou filosofia enquanto pensa sobre um problema em particular ou questão difícil que você enfrenta, e faça depois faça um teste de Religião (CD determinada pelo MJ). Se obtiver sucesso, você descobre uma passagem, parábola ou aforismo relevante que pode lhe ajudar a seguir adiante ou mudar seu pensamento para solucionar seu problema. Por exemplo, o MJ pode lhe fornecer uma dica ou poema enigmático que pode guiá-lo ao próximo passo para solucionar seu problema. </t>
+  </si>
+  <si>
+    <t>PASSO APRUMADO</t>
+  </si>
+  <si>
+    <t>Destreza 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você dá um passo rápida e cuidadosamente. Você pode Dar um Passo em terreno difícil. </t>
+  </si>
+  <si>
+    <t>PECHINCHADOR</t>
+  </si>
+  <si>
+    <t>Você pode Ganhar Proventos utilizando Diplomacia, gastando seus dias procurando barganhas e revendendo para gerar lucro. Você também pode gastar tempo especificamente procurando por uma boa barganha em um item; isto funciona como se você estivesse usando Ganhar Proventos com Diplomacia, exceto que em vez de ganhar dinheiro, compra o item com um desconto igual ao dinheiro que teria ganho, recebendo o item gratuitamente se seu ganho de proventos igualar ou exceder o custo dele. Finalmente, se selecionar Pechinchador durante a criação de personagem no 1º nível, você começa o jogo com 2 po adicionais.</t>
+  </si>
+  <si>
+    <t>PEDIDO DESAVERGONHADO</t>
+  </si>
+  <si>
+    <t>mestre em Diplomacia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você pode minimizar as consequência ou ultraje de seus pedidos usando puro charme e insolência. Quando Pedir alguma coisa, você reduz qualquer aumento na CD por fazer um pedido ultrajante em 2 pontos e, se rolar uma falha crítica para seu Pedido, trate o resultado como uma falha. Embora isto signifique que você nunca faz seu alvo piorar a atitude dele em relação ao você fazendo um Pedido, eventualmente ele se cansa de pedidos, mesmo que tenha uma atitude positiva em relação a você. </t>
+  </si>
+  <si>
+    <t>PERFORMANCE FASCINANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quando Performar, compare seu resultado à CD de Vontade de um observador. Se obtiver sucesso, o alvo fica fascinado por você por 1 rodada. Se o observador estiver em uma situação que exige atenção imediata, tal como um combate, você deve obter um sucesso crítico para fasciná-lo e a ação Performar adquire o traço incapacitação. Você deve escolher qual criatura está tentando fascinar antes de rolar seu teste, e depois o alvo fica temporariamente imune por 1 hora. Se for especialista em Performance, você pode fascinar até quatro observadores; se for mestre em Performance, pode fascinar até 10 observadores; e se for lendário em Performance, pode fascinar qualquer quantidade de observadores ao mesmo tempo. </t>
+  </si>
+  <si>
+    <t>PERFORMANCE IMPRESSIONANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suas performances inspiram admiração e lhe garante fãs. Você pode Impressionar utilizando Performance em vez de Diplomacia. </t>
+  </si>
+  <si>
+    <t>PERSPICÁCIA SAGAZ</t>
+  </si>
+  <si>
+    <t>Sua capacidade de evitar algo ou sua observação está além do comum para a maioria em sua profissão. Escolha salvamentos de Fortitude, Reflexos ou Vontade, ou Percepção. Você se torna especialista em sua escolha. No 17º nível, você se torna mestre em sua escolha.</t>
+  </si>
+  <si>
+    <t>POLIGLOTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você entende facilmente novos idiomas. Você aprende dois novos idiomas, escolhidos dentre os idiomas comuns, idiomas incomuns e quaisquer outros idiomas aos quais tenha acesso. Você aprende um idioma adicional se for ou se tornar mestre em Sociedade e novamente se for ou se tornar lendário. Especial Você pode selecionar este talento várias vezes. Cada vez que o fizer, você aprende idiomas adicionais. </t>
+  </si>
+  <si>
+    <t>PROCURA ACELERADA</t>
+  </si>
+  <si>
+    <t>mestre em Percepção</t>
+  </si>
+  <si>
+    <t>Você possui um sistema que lhe permite procurar em grande velocidade, encontrando detalhes e segredos duas vezes mais rápido do que outros poderiam. Quando Procurar, você leva metade do tempo usual para Procurar em uma determinada área. Isto significa que, enquanto estiver explorando, você dobra a Velocidade em que pode se mover enquanto Procura em uma área antes de andar nela (até metade de sua Velocidade). Se for lendário em Percepção, em vez disso você pode Procurar quatro vezes mais rápido quando escolher uma área.</t>
+  </si>
+  <si>
+    <t>PROCURAR VIDA SELVAGEM</t>
+  </si>
+  <si>
+    <t>Você pode estudar detalhes nos ermos para determinar a presença de criaturas próximas. Você pode gastar 10 minutos aferindo a área ao seu redor para descobrir quais criaturas há por perto, baseado em ninhos, excrementos e marcas na vegetação. Faça um teste de Sobrevivência contra a CD determinada pelo MJ baseado em quão óbvios são os sinais. Em um sucesso, você pode fazer um teste de Recordar Conhecimento com –2 de penalidade para aprender mais sobre as criaturas somente a partir destes sinais. Se for mestre em Sobrevivência, você não sofre a penalidade.</t>
+  </si>
+  <si>
+    <t>PROEZA INTIMIDANTE</t>
+  </si>
+  <si>
+    <t>Força 16, especialista em Intimidação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Em situações onde você pode ameaçar o alvo fisicamente quando Coagir ou Desmoralizar, você recebe +1 de bônus de circunstância em seu teste de Intimidação e ignora a penalidade por não compartilhar um idioma. Se seu valor de Força for 20 ou maior e você for mestre em Intimidação, este bônus aumenta para +2. </t>
+  </si>
+  <si>
+    <t>PROFICIÊNCIA COM ARMAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você se torna treinado em todas as armas simples. Se já for treinado em todas as armas simples, você recebe treinamento em todas as armas marciais. Se já for treinado em todas as armas simples e marciais, você recebe treinamento em uma arma avançada à sua escolha. Especial Você pode selecionar este talento várias vezes. Cada vez que o fizer, você se torna treinado no próximo tipo de arma, seguindo a progressão acima. </t>
+  </si>
+  <si>
+    <t>PROFICIÊNCIA COM ARMADURAS</t>
+  </si>
+  <si>
+    <t>Você se torna treinado em armaduras leves. Se já for treinado em armaduras leves, você recebe treinamento em armaduras médias. Se já for treinado em armaduras leves e médias, você recebe treinamento em armaduras pesadas. Especial Você pode selecionar este talento várias vezes. Cada vez que o fizer, você se torna treinado no próximo tipo de armadura, seguindo a progressão acima.</t>
+  </si>
+  <si>
+    <t>PROFISSIONAL EXPERIENTE</t>
+  </si>
+  <si>
+    <t>treinado em Saber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você salvaguarda cuidadosamente suas empreitadas profissionais para evitar desastres. Quando usar Saber para Ganhar Proventos, se rolar uma falha crítica, trate o resultado como uma falha. Se for especialista em Saber, você ganha o dobro de proventos de um teste que tenha falhado para Ganhar Proventos, a menos que originalmente o resultado fosse uma falha crítica. </t>
+  </si>
+  <si>
+    <t>PROFISSIONAL LENDÁRIO</t>
+  </si>
+  <si>
+    <t>lendário em Saber</t>
+  </si>
+  <si>
+    <t>Sua fama se espalhou pelas terras (se tiver Saber de Guerra, por exemplo, você pode ser um tático ou general lendário). Isto funciona como Artista Lendário, exceto que você consegue trabalhos de níveis superiores quando Ganhar Proventos com Saber.</t>
+  </si>
+  <si>
+    <t>PUNGA</t>
+  </si>
+  <si>
+    <t>Você pode Furtar ou Empalmar um Objeto que esteja bem guardado, como em um bolso, sem sofrer os –5 de penalidade normais. Você não pode furtar objetos que seriam extremamente perceptíveis ou que consumam tempo para remover (como sapatos calçados, armaduras vestidas ou objetos ativamente empunhados). Se for mestre em Ladroagem, você pode tentar Furtar de uma criatura que esteja em combate ou em guarda. Quando o fizer, Furtar requer 2 ações de manuseio em vez de 1, e você sofre –5 de penalidade.</t>
+  </si>
+  <si>
+    <t>QUEDA DO GATO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suas acrobacias aéreas felinas permitem que você amorteça suas quedas. Trate quedas como 3 metros mais curtas. Se for especialista em Acrobatismo, trate quedas como 7,5 metros mais curtas. Se for mestre em Acrobatismo, trate quedas como 15 metros mais curtas. Se for lendário em Acrobatismo, você sempre cai de pé e não sofre dano, independentemente da distância da queda. </t>
+  </si>
+  <si>
+    <t>RASTEJO LIGEIRO</t>
+  </si>
+  <si>
+    <t>especialista em Acrobatismo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você pode Rastejar incrivelmente rápido — até metade de sua Velocidade, em vez de 1,5 metros. Se for mestre em Acrobatismo, você pode Rastejar à sua Velocidade total e, se for lendário, você não fica desprevenido enquanto estiver prostrado. </t>
+  </si>
+  <si>
+    <t>RASTREADOR EXPERIENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rastrear está enraizado em sua natureza e, quando necessário, você pode seguir uma trilha sem hesitar. Você pode Rastrear enquanto se move à sua Velocidade total ao sofrer –5 de penalidade em seu teste de Sobrevivência. Se for mestre em Sobrevivência, você não sofre os –5 de penalidade. Se for lendário em Sobrevivência, você não precisa mais rolar um novo teste de Sobrevivência a cada hora em que estiver rastreando, embora ainda precise rolar sempre que houver mudanças significativas na trilha. </t>
+  </si>
+  <si>
+    <t>RECONHECER MAGIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acionamento: Uma criatura em sua linha de visão conjura uma magia que você não possui preparada ou em seu repertório de magias, ou uma armadilha ou objeto similar conjura uma magia dessas. Você deve estar ciente da conjuração. Se for treinado na perícia apropriada para a tradição da magia e ela for uma magia comum de 2º nível ou inferior, você a identifica automaticamente (você ainda precisa rolar para tentar obter um sucesso crítico, mas não obtém um resultado pior do que um sucesso). O nível mais alto de magia que pode identificar automaticamente aumenta para 4 se você for especialista, 6 se for mestre e 10 se for lendário. O MJ rola um teste secreto de Arcanismo, Natureza, Ocultismo ou Religião (o que corresponder à tradição da magia sendo conjurada). Se você não for treinado na perícia, você não pode obter um resultado melhor que uma falha. Sucesso Crítico: Você reconhece corretamente a magia e recebe +1 de bônus de circunstância em sua jogada de salvamento ou CA contra essa magia. Sucesso: Você reconhece corretamente a magia. Falha Você falha: em reconhecer a magia. Falha Crítica: Você identifica a magia erroneamente como outra magia completamente diferente à escolha do MJ. </t>
+  </si>
+  <si>
+    <t>RECONHECIMENTO RÁPIDO</t>
+  </si>
+  <si>
+    <t>mestre em Arcanismo, Natureza, Ocultismo ou Religião; Reconhecer Magia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você Reconhece Magias rapidamente. Uma vez por rodada, você pode Reconhecer uma Magia utilizando uma perícia na qual você seja mestre como uma ação livre. </t>
+  </si>
+  <si>
+    <t>RECUPERAÇÃO CONTÍNUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você monitora zelosamente o progresso de um paciente para administrar um tratamento mais rápido. Quando você Tratar Ferimentos, seu paciente fica imune por apenas 10 minutos em vez de por 1 hora. Isto se aplica somente às suas atividades de Tratar Ferimentos, não a qualquer outra que o paciente receber. </t>
+  </si>
+  <si>
+    <t>RECUPERAÇÃO RÁPIDA</t>
+  </si>
+  <si>
+    <t>Constituição 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seu corpo combate aflições rapidamente. Você recupera o dobro de Pontos de Vida por descansar. Cada vez que obtiver sucesso em um salvamento de Fortitude contra uma doença ou veneno em efeito, você reduz seu estágio em 2, ou em 1 contra uma doença ou veneno virulento. Cada sucesso crítico que você obtiver contra uma doença ou veneno em efeito reduz seu estágio em 3, ou em 2 contra uma doença ou veneno virulento. Além disso, você reduz a severidade de sua condição drenado em 2 quanto descansar por uma noite em vez de reduzi-la em 1. </t>
+  </si>
+  <si>
+    <t>RECUPERAÇÃO ROBUSTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você aprendeu medicina popular para ajudar a recuperar de doenças e venenos, e usá-la diligentemente o tornou especialmente resiliente. Quando você Tratar uma Doença ou Veneno, ou quando alguém usar uma destas ações em você, aumente o bônus de circunstância concedido em um sucesso para +4, e se o resultado da jogada de salvamento do paciente for um sucesso, o paciente trata o resultado como um sucesso crítico. </t>
+  </si>
+  <si>
+    <t>REPARO RÁPIDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você leva 1 minuto para Reparar um item. Se for mestre em Manufatura, isso leva 3 ações. Se for lendário em Manufatura, isso leva 1 ação. </t>
+  </si>
+  <si>
+    <t>RETIRADA ATERRORIZADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quando obtiver um sucesso crítico na ação Desmoralizar, se o nível do alvo for menor que o seu, o alvo fica fugindo por 1 rodada. </t>
+  </si>
+  <si>
+    <t>SABER ADICIONAL</t>
+  </si>
+  <si>
+    <t>Seu conhecimento expandiu para abranger um novo campo. Escolha uma subcategoria adicional da perícia Saber. Você se torna treinado nela. No 3º, 7º e 15º níveis, você recebe um incremento de perícia adicional que você pode aplicar somente à subcategoria escolhida de Saber. Especial Você pode selecionar este talento várias vezes. Cada vez que o fizer, você deve selecionar uma nova subcategoria de Saber e recebe os incrementos de perícia adicionais para essa subcategoria nos níveis listados.</t>
+  </si>
+  <si>
+    <t>SABER INCONFUNDÍVEL</t>
+  </si>
+  <si>
+    <t>especialista em Saber</t>
+  </si>
+  <si>
+    <t>Você nunca obtém informações errôneas sobre suas áreas de especialidade. Quando Recordar Conhecimento utilizando qualquer subcategoria de Saber na qual é treinado, se rolar uma falha crítica, trate o resultado como falha. Se for mestre em uma subcategoria de Saber, em um sucesso crítico, você obtém ainda mais informações ou contexto do que o usual.</t>
+  </si>
+  <si>
+    <t>SALTO NAS NUVENS</t>
+  </si>
+  <si>
+    <t>lendário em Atletismo</t>
+  </si>
+  <si>
+    <t>Sua capacidade atlética inigualável lhe permite saltar distâncias impossíveis. Triplique a distância de seu Salto em Distância (portanto, você poderia saltar 18 metros em um teste bem-sucedido de CD 20). Quando Saltar em Altura, use o cálculo para Salto em Distância, mas não triplique a distância. Quando Saltar em Altura ou Saltar em Distância, você também pode aumentar a quantidade de ações que usar (até a quantidade de ações remanescentes em seu turno) para saltar ainda mais longe. Para cada ação extra, adicione sua Velocidade à distância máxima que você salta.</t>
+  </si>
+  <si>
+    <t>SALTO NA PAREDE</t>
+  </si>
+  <si>
+    <t>Você pode usar seu impulso de um salto para propelir-se de uma parede. Se estiver adjacente a uma parede ao final de um salto (seja realizando um Salto, Salto em Altura ou Salto em Distância), você não cai desde que sua próxima ação seja outro salto. Além disso, como seu salto prévio lhe dá impulso, você pode usar Salto em Altura ou Salto em Distância como uma ação única, mas você não Anda como parte da atividade. Você pode usar Salto na Parede somente uma vez por turno, a menos que seja lendário em Atletismo, sendo que nesse caso você pode Saltar na Parede tantas vezes quanto puder usar ações consecutivas nesse turno.</t>
+  </si>
+  <si>
+    <t>SALTO PODEROSO</t>
+  </si>
+  <si>
+    <t>especialista em Atletismo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quando Saltar, você pode Saltar até 1,5 metros em um Salto vertical e aumenta a distância que pode saltar horizontalmente em 1,5 metros. </t>
+  </si>
+  <si>
+    <t>SALTO RÁPIDO</t>
+  </si>
+  <si>
+    <t>Você pode usar Salto em Altura ou Salto em Distância como uma ação única em vez de 2 ações. Se o fizer, você não realiza o Andar inicial (nem falha se não Andar 3 metros).</t>
+  </si>
+  <si>
+    <t>SAQUEADOR SUBAQUÁTICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você aprendeu a lutar embaixo d’água. Você não fica desprevenido enquanto estiver na água, e não sofre as penalidades normais por usar uma arma corpo a corpo contundente ou cortante na água. </t>
+  </si>
+  <si>
+    <t>SEGREDOS ESCORREGADIOS</t>
+  </si>
+  <si>
+    <t>mestre em Dissimulação</t>
+  </si>
+  <si>
+    <t>Você engana e evita tentativas de descobrir sua verdadeira natureza ou suas intenções. Quando uma magia ou efeito mágico tentar ler sua mente, detectar se você está mentindo ou revelar sua tendência, você pode fazer um teste de Dissimulação contra a CD da magia ou efeito. Se obtiver sucesso neste teste, o efeito não revela nada.</t>
+  </si>
+  <si>
+    <t>SEGURAR-SE RAPIDAMENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você pode facilmente se puxar em beiradas. Quando Segurar Numa Beirada, você pode se puxar em uma superfície e se levantar. Você pode utilizar Atletismo em vez de Reflexos para Segurar numa Beirada. </t>
+  </si>
+  <si>
+    <t>SENTIDO ARCANO</t>
+  </si>
+  <si>
+    <t>treinado em Arcanismo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seu estudo da magia permite que você sinta a presença dela instintivamente. Você pode conjurar detectar magia de 1º nível à vontade, como uma magia arcana inata. Se for mestre em Arcanismo, a magia é elevada para o 3º nível; se for lendário, a magia é elevada para o 4º nível. </t>
+  </si>
+  <si>
+    <t>SOBREVIVÊNCIA PLANAR</t>
+  </si>
+  <si>
+    <t>mestre em Sobrevivência</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você pode Subsistir utilizando Sobrevivência em planos diferentes, mesmo naqueles sem recursos ou fenômenos naturais que você normalmente precise. Por exemplo, você pode forragear por comida até mesmo em planos que não tenham comida que normalmente o sustentaria. Um sucesso em seu teste para Subsistir também pode reduzir o dano causado pelo plano, a critério do MJ. </t>
+  </si>
+  <si>
+    <t>SOBREVIVENTE LENDÁRIO</t>
+  </si>
+  <si>
+    <t>lendário em Sobrevivência</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você pode sobrevier indefinidamente sem comida ou água e pode tolerar calor ou frio severos, extremos e incríveis sem sofrer dano por isso. </t>
+  </si>
+  <si>
+    <t>TEORIA UNIFICADA</t>
+  </si>
+  <si>
+    <t>lendário em Arcanismo</t>
+  </si>
+  <si>
+    <t>Você começou a formar uma conexão significativa sobre os fundamentos comuns das quatro tradições de magia e essências mágicas, permitindo-lhe compreender todas elas através de uma visão arcana. Sempre que você usar uma ação ou talento de perícia que requeira um teste de Natureza, Ocultismo ou Religião, dependendo da tradição mágica, você pode utilizar Arcanismo em vez dessas perícias. Se normalmente fosse sofrer uma penalidade ou rolar contra uma CD maior por utilizar Arcanismo para outras magias (como quando usar Identificar Magia), isso não ocorre mais.</t>
+  </si>
+  <si>
+    <t>TREINAMENTO EM PERÍCIA</t>
+  </si>
+  <si>
+    <t>Inteligência 12</t>
+  </si>
+  <si>
+    <t>Você se torna treinado em uma perícia à sua escolha. Especial Você pode selecionar este talento várias vezes. Cada vez que o fizer, você deve selecionar uma nova perícia para se tornar treinado.</t>
+  </si>
+  <si>
+    <t>TREINAR ANIMAL</t>
+  </si>
+  <si>
+    <t>Você passa tempo ensinando um animal para fazer uma certa ação. Você pode selecionar uma ação básica que o animal já saiba como fazer (geralmente uma das listadas na ação Comandar um Animal) ou tentar ensinar uma nova ação básica ao animal. O MJ determina a CD de qualquer teste necessário e a quantidade de tempo que o treinamento leva (normalmente pelo menos uma semana). Normalmente é impossível ensinar a um animal um truque que exija pensamento crítico. Se for especialista, mestre ou lendário em Natureza, você pode ser capaz de treinar criaturas mais inusitadas, a critério do MJ. Sucesso O animal aprende a ação. Se fosse uma ação que o animal já conhecia, você pode Comandar o Animal a fazer essa ação sem fazer um teste de Natureza. Se fosse uma ação básica nova, acrescente essa ação às ações que o animal pode realizar quando Comandado, mas ainda deve fazer a rolagem. Falha O animal não aprende o truque.</t>
+  </si>
+  <si>
+    <t>VELOZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você se move mais rápido a pé. Sua Velocidade aumenta em 1,5 metros. </t>
+  </si>
+  <si>
+    <t>VITALIDADE</t>
+  </si>
+  <si>
+    <t>Você pode suportar mais punição que a maioria antes de sucumbir. Aumente seus Pontos de Vida máximos em uma quantidade igual ao seu nível. Você reduz a CD de testes de recuperação em 1 ponto.</t>
+  </si>
+  <si>
+    <t>Atividade de Três Ações</t>
+  </si>
+  <si>
+    <t>SECRETO</t>
   </si>
 </sst>
 </file>
@@ -926,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,1336 +1301,2312 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
         <v>15</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="C5" t="s">
+        <v>20</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
-        <v>70</v>
-      </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B25">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
-        <v>89</v>
-      </c>
       <c r="E28" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F29" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" t="s">
         <v>93</v>
       </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" t="s">
-        <v>9</v>
-      </c>
       <c r="H30" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E31" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>100</v>
-      </c>
-      <c r="H31" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B32">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F32" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F33" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G33" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="E35" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F35" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B36">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F36" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F37" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B38">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F38" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E39" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G39" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F40" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F41" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G41" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>128</v>
+        <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F42" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>116</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F43" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="G43" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E44" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F44" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E45" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F45" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="E46" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F46" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="E47" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F47" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="E48" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F48" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F49" t="s">
-        <v>8</v>
-      </c>
-      <c r="G49" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F50" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>145</v>
       </c>
       <c r="E51" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F51" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="G51" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B52">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E52" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F52" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" t="s">
-        <v>9</v>
-      </c>
-      <c r="H52" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B53">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E53" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F53" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="G53" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B54">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="E54" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F54" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G54" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>158</v>
       </c>
       <c r="D55" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="E55" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F55" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G55" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B56">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s">
-        <v>165</v>
+        <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="E56" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F56" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G56" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="E57" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F57" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G57" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B58">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>169</v>
+        <v>34</v>
       </c>
       <c r="E58" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F58" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G58" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D59" t="s">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="E59" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F59" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G59" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B60">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="E60" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F60" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G60" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="E61" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F61" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G61" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E62" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F62" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G62" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D63" t="s">
-        <v>120</v>
+        <v>176</v>
       </c>
       <c r="E63" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F63" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E64" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F64" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G64" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D65" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E65" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F65" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G65" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B66">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
       </c>
       <c r="D66" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E66" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F66" t="s">
-        <v>8</v>
+        <v>187</v>
       </c>
       <c r="G66" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="H66" t="s">
+        <v>93</v>
+      </c>
+      <c r="I66" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>188</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>189</v>
+      </c>
+      <c r="E67" t="s">
+        <v>190</v>
+      </c>
+      <c r="F67" t="s">
+        <v>3</v>
+      </c>
+      <c r="G67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>191</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
-        <v>26</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
         <v>192</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E68" t="s">
         <v>193</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F68" t="s">
+        <v>3</v>
+      </c>
+      <c r="G68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>194</v>
       </c>
-      <c r="G67" t="s">
-        <v>8</v>
-      </c>
-      <c r="H67" t="s">
-        <v>100</v>
-      </c>
-      <c r="I67" t="s">
-        <v>9</v>
+      <c r="B69">
+        <v>15</v>
+      </c>
+      <c r="D69" t="s">
+        <v>195</v>
+      </c>
+      <c r="E69" t="s">
+        <v>196</v>
+      </c>
+      <c r="F69" t="s">
+        <v>3</v>
+      </c>
+      <c r="G69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>197</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>82</v>
+      </c>
+      <c r="E70" t="s">
+        <v>198</v>
+      </c>
+      <c r="F70" t="s">
+        <v>3</v>
+      </c>
+      <c r="G70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>199</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>82</v>
+      </c>
+      <c r="E71" t="s">
+        <v>200</v>
+      </c>
+      <c r="F71" t="s">
+        <v>3</v>
+      </c>
+      <c r="G71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>201</v>
+      </c>
+      <c r="B72">
+        <v>7</v>
+      </c>
+      <c r="D72" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72" t="s">
+        <v>202</v>
+      </c>
+      <c r="F72" t="s">
+        <v>3</v>
+      </c>
+      <c r="G72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>203</v>
+      </c>
+      <c r="B73">
+        <v>15</v>
+      </c>
+      <c r="C73" t="s">
+        <v>313</v>
+      </c>
+      <c r="D73" t="s">
+        <v>204</v>
+      </c>
+      <c r="E73" t="s">
+        <v>205</v>
+      </c>
+      <c r="F73" t="s">
+        <v>3</v>
+      </c>
+      <c r="G73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>49</v>
+      </c>
+      <c r="E74" t="s">
+        <v>207</v>
+      </c>
+      <c r="F74" t="s">
+        <v>3</v>
+      </c>
+      <c r="G74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>208</v>
+      </c>
+      <c r="B75">
+        <v>15</v>
+      </c>
+      <c r="D75" t="s">
+        <v>209</v>
+      </c>
+      <c r="E75" t="s">
+        <v>210</v>
+      </c>
+      <c r="F75" t="s">
+        <v>3</v>
+      </c>
+      <c r="G75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>211</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>212</v>
+      </c>
+      <c r="E76" t="s">
+        <v>213</v>
+      </c>
+      <c r="F76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>214</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>31</v>
+      </c>
+      <c r="E77" t="s">
+        <v>215</v>
+      </c>
+      <c r="F77" t="s">
+        <v>3</v>
+      </c>
+      <c r="G77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>216</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="D78" t="s">
+        <v>217</v>
+      </c>
+      <c r="E78" t="s">
+        <v>218</v>
+      </c>
+      <c r="F78" t="s">
+        <v>3</v>
+      </c>
+      <c r="G78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>219</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" t="s">
+        <v>220</v>
+      </c>
+      <c r="F79" t="s">
+        <v>3</v>
+      </c>
+      <c r="G79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>221</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" t="s">
+        <v>222</v>
+      </c>
+      <c r="F80" t="s">
+        <v>3</v>
+      </c>
+      <c r="G80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>223</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>224</v>
+      </c>
+      <c r="F81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>225</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>131</v>
+      </c>
+      <c r="E82" t="s">
+        <v>226</v>
+      </c>
+      <c r="F82" t="s">
+        <v>3</v>
+      </c>
+      <c r="G82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>227</v>
+      </c>
+      <c r="B83">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>228</v>
+      </c>
+      <c r="E83" t="s">
+        <v>229</v>
+      </c>
+      <c r="F83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>230</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>116</v>
+      </c>
+      <c r="E84" t="s">
+        <v>231</v>
+      </c>
+      <c r="F84" t="s">
+        <v>3</v>
+      </c>
+      <c r="G84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>232</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s">
+        <v>233</v>
+      </c>
+      <c r="E85" t="s">
+        <v>234</v>
+      </c>
+      <c r="F85" t="s">
+        <v>3</v>
+      </c>
+      <c r="G85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>235</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>236</v>
+      </c>
+      <c r="F86" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>237</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>238</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>239</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="D88" t="s">
+        <v>240</v>
+      </c>
+      <c r="E88" t="s">
+        <v>241</v>
+      </c>
+      <c r="F88" t="s">
+        <v>3</v>
+      </c>
+      <c r="G88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>242</v>
+      </c>
+      <c r="B89">
+        <v>15</v>
+      </c>
+      <c r="D89" t="s">
+        <v>243</v>
+      </c>
+      <c r="E89" t="s">
+        <v>244</v>
+      </c>
+      <c r="F89" t="s">
+        <v>3</v>
+      </c>
+      <c r="G89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>245</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>128</v>
+      </c>
+      <c r="E90" t="s">
+        <v>246</v>
+      </c>
+      <c r="F90" t="s">
+        <v>3</v>
+      </c>
+      <c r="G90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>247</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>98</v>
+      </c>
+      <c r="E91" t="s">
+        <v>248</v>
+      </c>
+      <c r="F91" t="s">
+        <v>3</v>
+      </c>
+      <c r="G91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>249</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
+        <v>250</v>
+      </c>
+      <c r="E92" t="s">
+        <v>251</v>
+      </c>
+      <c r="F92" t="s">
+        <v>3</v>
+      </c>
+      <c r="G92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>252</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>116</v>
+      </c>
+      <c r="E93" t="s">
+        <v>253</v>
+      </c>
+      <c r="F93" t="s">
+        <v>3</v>
+      </c>
+      <c r="G93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>254</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>25</v>
+      </c>
+      <c r="D94" t="s">
+        <v>91</v>
+      </c>
+      <c r="E94" t="s">
+        <v>255</v>
+      </c>
+      <c r="F94" t="s">
+        <v>3</v>
+      </c>
+      <c r="G94" t="s">
+        <v>4</v>
+      </c>
+      <c r="H94" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>256</v>
+      </c>
+      <c r="B95">
+        <v>7</v>
+      </c>
+      <c r="D95" t="s">
+        <v>257</v>
+      </c>
+      <c r="E95" t="s">
+        <v>258</v>
+      </c>
+      <c r="F95" t="s">
+        <v>3</v>
+      </c>
+      <c r="G95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>259</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="D96" t="s">
+        <v>192</v>
+      </c>
+      <c r="E96" t="s">
+        <v>260</v>
+      </c>
+      <c r="F96" t="s">
+        <v>3</v>
+      </c>
+      <c r="G96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>261</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>262</v>
+      </c>
+      <c r="E97" t="s">
+        <v>263</v>
+      </c>
+      <c r="F97" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>264</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>192</v>
+      </c>
+      <c r="E98" t="s">
+        <v>265</v>
+      </c>
+      <c r="F98" t="s">
+        <v>3</v>
+      </c>
+      <c r="G98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>266</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>113</v>
+      </c>
+      <c r="E99" t="s">
+        <v>267</v>
+      </c>
+      <c r="F99" t="s">
+        <v>3</v>
+      </c>
+      <c r="G99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>268</v>
+      </c>
+      <c r="B100">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>28</v>
+      </c>
+      <c r="E100" t="s">
+        <v>269</v>
+      </c>
+      <c r="F100" t="s">
+        <v>3</v>
+      </c>
+      <c r="G100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>270</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>240</v>
+      </c>
+      <c r="E101" t="s">
+        <v>271</v>
+      </c>
+      <c r="F101" t="s">
+        <v>3</v>
+      </c>
+      <c r="G101" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>272</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s">
+        <v>273</v>
+      </c>
+      <c r="E102" t="s">
+        <v>274</v>
+      </c>
+      <c r="F102" t="s">
+        <v>3</v>
+      </c>
+      <c r="G102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>275</v>
+      </c>
+      <c r="B103">
+        <v>15</v>
+      </c>
+      <c r="D103" t="s">
+        <v>276</v>
+      </c>
+      <c r="E103" t="s">
+        <v>277</v>
+      </c>
+      <c r="F103" t="s">
+        <v>3</v>
+      </c>
+      <c r="G103" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>278</v>
+      </c>
+      <c r="B104">
+        <v>7</v>
+      </c>
+      <c r="D104" t="s">
+        <v>101</v>
+      </c>
+      <c r="E104" t="s">
+        <v>279</v>
+      </c>
+      <c r="F104" t="s">
+        <v>3</v>
+      </c>
+      <c r="G104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>280</v>
+      </c>
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s">
+        <v>281</v>
+      </c>
+      <c r="E105" t="s">
+        <v>282</v>
+      </c>
+      <c r="F105" t="s">
+        <v>3</v>
+      </c>
+      <c r="G105" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>283</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="D106" t="s">
+        <v>34</v>
+      </c>
+      <c r="E106" t="s">
+        <v>284</v>
+      </c>
+      <c r="F106" t="s">
+        <v>3</v>
+      </c>
+      <c r="G106" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>285</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="D107" t="s">
+        <v>34</v>
+      </c>
+      <c r="E107" t="s">
+        <v>286</v>
+      </c>
+      <c r="F107" t="s">
+        <v>3</v>
+      </c>
+      <c r="G107" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>287</v>
+      </c>
+      <c r="B108">
+        <v>7</v>
+      </c>
+      <c r="D108" t="s">
+        <v>288</v>
+      </c>
+      <c r="E108" t="s">
+        <v>289</v>
+      </c>
+      <c r="F108" t="s">
+        <v>3</v>
+      </c>
+      <c r="G108" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>290</v>
+      </c>
+      <c r="B109">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>281</v>
+      </c>
+      <c r="E109" t="s">
+        <v>291</v>
+      </c>
+      <c r="F109" t="s">
+        <v>3</v>
+      </c>
+      <c r="G109" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>292</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>293</v>
+      </c>
+      <c r="E110" t="s">
+        <v>294</v>
+      </c>
+      <c r="F110" t="s">
+        <v>3</v>
+      </c>
+      <c r="G110" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>295</v>
+      </c>
+      <c r="B111">
+        <v>7</v>
+      </c>
+      <c r="D111" t="s">
+        <v>296</v>
+      </c>
+      <c r="E111" t="s">
+        <v>297</v>
+      </c>
+      <c r="F111" t="s">
+        <v>3</v>
+      </c>
+      <c r="G111" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>298</v>
+      </c>
+      <c r="B112">
+        <v>15</v>
+      </c>
+      <c r="D112" t="s">
+        <v>299</v>
+      </c>
+      <c r="E112" t="s">
+        <v>300</v>
+      </c>
+      <c r="F112" t="s">
+        <v>3</v>
+      </c>
+      <c r="G112" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>301</v>
+      </c>
+      <c r="B113">
+        <v>15</v>
+      </c>
+      <c r="D113" t="s">
+        <v>302</v>
+      </c>
+      <c r="E113" t="s">
+        <v>303</v>
+      </c>
+      <c r="F113" t="s">
+        <v>3</v>
+      </c>
+      <c r="G113" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>304</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="D114" t="s">
+        <v>305</v>
+      </c>
+      <c r="E114" t="s">
+        <v>306</v>
+      </c>
+      <c r="F114" t="s">
+        <v>3</v>
+      </c>
+      <c r="G114" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>307</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="D115" t="s">
+        <v>189</v>
+      </c>
+      <c r="E115" t="s">
+        <v>308</v>
+      </c>
+      <c r="F115" t="s">
+        <v>3</v>
+      </c>
+      <c r="G115" t="s">
+        <v>93</v>
+      </c>
+      <c r="H115" t="s">
+        <v>4</v>
+      </c>
+      <c r="I115" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>309</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
+        <v>310</v>
+      </c>
+      <c r="F116" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>311</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="E117" t="s">
+        <v>312</v>
+      </c>
+      <c r="F117" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionados talentos de Alquimista
</commit_message>
<xml_diff>
--- a/data/talentos.xlsx
+++ b/data/talentos.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="talentos" sheetId="1" r:id="rId1"/>
+    <sheet name="gerais" sheetId="1" r:id="rId1"/>
+    <sheet name="classes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="403">
   <si>
     <t>especialista em Furtividade</t>
   </si>
@@ -969,6 +970,270 @@
   </si>
   <si>
     <t>ALIADOS QUIETOS</t>
+  </si>
+  <si>
+    <t>BOMBARDEIRO RÁPIDO</t>
+  </si>
+  <si>
+    <t>Você guarda suas bombas em bolsos fáceis de alcançar de onde consegue pegá-las sem pensar. Você Interage para sacar uma bomba e Golpear com ela.</t>
+  </si>
+  <si>
+    <t>ALQUIMISTA</t>
+  </si>
+  <si>
+    <t>FAMILIAR ALQUÍMICO</t>
+  </si>
+  <si>
+    <t>Você consegue criar vida através da alquimia — uma criatura simples formada a partir demateriais alquímicos, reagentes e um pouco de seu próprio sangue. Este familiar alquímicoparece ser uma pequena criatura de carne e sangue, embora possa ter algumas característicasinusitadas ou distintas dependendo de seu processo criativo. Como outros familiares, seufamiliar alquímico o ajuda em seu laboratório e em suas aventuras. Você utiliza seu própriomodificador de Inteligência para determinar os modificadores de Percepção, Acrobatismo eFurtividade do familiar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAPIENTE ALQUÍMICO </t>
+  </si>
+  <si>
+    <t>Pré-requisitos treinado em Manufatura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você consegue identificar itens alquímicos rapidamente. Quando usar a perícia Manufatura para Identificar Alquimia em um item alquímico que estiver segurando, você pode fazê-lo como uma ação única que possui os traços concentração e manuseio (em vez de gastar 10 minutos). Se tiver a fórmula do item sendo identificado, você recebe +2 de bônus de circunstância em seu teste, e se rolar uma falha crítica, trate o resultado como uma falha. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANÇADOR LONGÍNQUO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você aprendeu a arremessar mais longe. Quando você arremessa uma bomba alquímica, ela possui um incremento de distância de 9 metros em vez dos 6 metros usuais. </t>
+  </si>
+  <si>
+    <t>BOMBA DE FUMAÇA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequência uma vez por rodada Acionamento Você usa Alquimia Rápida para manufaturar uma bomba alquímica com nível de item pelo menos 1 nível inferior ao seu nível de alquimia avançada. Você faz a bomba criar uma nuvem de fumaça espessa além de seus efeitos normais. Quando arremessada, a bomba cria uma nuvem de fumaça em uma explosão de 3 metros de raio. A nuvem é centralizada em um canto à sua escolha no espaço do alvo (ou no espaço onde a bomba aterrissar). Criaturas dentro dessa área recebem a condição ocultada, e todas as outras criaturas estão ocultadas contra elas. A fumaça dura por 1 minuto ou até ser dissipada por um vento forte. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADITIVO 1 </t>
+  </si>
+  <si>
+    <t>MUTAGÊNICO REVIVIFICANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enquanto estiver sob efeito de um mutagênico, você pode metabolizar o poder do mutagênico para se curar. Para isso, você usa uma ação única que possui os traços concentração e manuseio. Assim que a ação é completada, você recupera 1d6 Pontos de Vida para cada 2 níveis de item do mutagênico (mínimo 1d6), mas a duração do mutagênico é encerrada imediatamente (mesmo se estiver sob o efeito de Mutagênico Persistente). </t>
+  </si>
+  <si>
+    <t>RESISTÊNCIA A VENENO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A exposição constante a reagentes tóxicos fortificou seu corpo contra venenos de todos os tipos. Você recebe resistência a veneno igual à metade de seu nível, e recebe +1 de bônus de estado em jogadas de salvamento contra venenos. </t>
+  </si>
+  <si>
+    <t>ALQUIMIA DURADOURA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você aprendeu a fazer sua energia pessoal durar um pouco mais quando prepara rapidamente suas concocções. Quando usar Alquimia Rápida para criar uma ferramenta ou elixir alquímico, essa ferramenta ou elixir permanece potente até o final de seu próximo turno (em vez de perder sua potência no início de seu próximo turno). </t>
+  </si>
+  <si>
+    <t>ALQUIMIA EFICIENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graças ao tempo passado em estudos e experimentos, você sabe como extrapolar suas fórmulas para lotes maiores que não requerem qualquer atenção adicional. Quando gastar tempo em recesso para Manufaturar itens alquímicos, você pode produzir o dobro de itens alquímicos em um único lote sem gastar qualquer tempo adicional de preparação. Por exemplo: se estiver criando elixires da vida, você pode manufaturar até oito elixires, em vez de quatro, em um único lote durante o recesso. Isto não reduz a quantidade de reagentes alquímicos requeridos ou outros ingredientes necessários para manufaturar cada item, nem aumenta sua velocidade de progresso para dias gastos além do recesso base. Isto também não altera a quantidade de itens que você pode criar em um lote usando alquimia avançada. </t>
+  </si>
+  <si>
+    <t>RESPINGO CALCULADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você calcula todos os ângulos para maximizar o respingo de uma bomba. Quando arremessar uma bomba alquímica com o traço respingo, você pode alterar o dano de respingo causado para que seja igual ao seu modificador de Inteligência (mínimo 0) em vez da quantidade normal de dano de respingo. </t>
+  </si>
+  <si>
+    <t>BOMBA DEBILITANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequência uma vez por rodada Acionamento Você usa Alquimia Rápida para manufaturar uma bomba alquímica com nível de item pelo menos 2 níveis inferior ao seu nível de alquimia avançada. Suas bombas impõem efeitos adicionais em seus inimigos. Você mistura uma substância na bomba que a faz causar um dos seguintes efeitos em seu alvo: desprevenido, ofuscado, surdo ou –1,5 metros de penalidade de estado em todas as Velocidades. Se o ataque com essa bomba acertar, o alvo deve obter sucesso em uma jogada de salvamento de Fortitude ou sofre esse efeito até o final de seu próximo turno. Utilize sua CD de classe para esta jogada de salvamento (mesmo se outra pessoa arremessar a bomba). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADITIVO 2 </t>
+  </si>
+  <si>
+    <t>BOMBAS DIRECIONAIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você consegue lançar bombas com grande força e uma trajetória precisa, angulando o respingo em um cone que jorra em uma única direção. Quando arremessar uma bomba alquímica com o traço respingo, em vez de respingar em todos os quadrados adjacentes ao alvo, você pode tratar o espaço do alvo como o primeiro quadrado afetado de um cone de 4,5 metros direcionado oposto a você — potencialmente permitindo-lhe evitar aliados e respingar mais à frente nas linhas inimigas. Se o alvo ocupar mais de um quadrado, o quadrado do alvo mais próximo de você é o primeiro afetado do cone. </t>
+  </si>
+  <si>
+    <t>COMBINAR ELIXIRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequência uma vez por rodada Acionamento Você usa Alquimia Rápida para manufaturar um item alquímico com o traço elixir com nível de item pelo menos 2 níveis inferior ao seu nível de alquimia avançada. Você descobriu como misturar dois elixires em uma única concocção híbrida. Você pode gastar 2 lotes adicionais de reagentes infundidos para acrescentar um segundo elixir ao que está sendo criado. O segundo elixir também deve ser pelo menos 2 níveis inferior ao seu nível de alquimia avançada, e o elixir combinado é um item alquímico dois níveis superior ao maior nível dentre os dois elixires combinados. Quando este elixir combinado é consumido, ambos os elixires constituintes surtem efeito. Por exemplo: você pode combinar dois elixires da vida para criar um elixir combinado que cura o dobro da quantidade normal ou pode combinar um elixir de visão no escuro menor com um elixir de olho de águia menor para receber visão no escuro e encontrar portas secretas. </t>
+  </si>
+  <si>
+    <t>ALQUIMIA PODEROSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Itens alquímicos que você cria na hora são particularmente potentes. Quando usar Alquimia Rápida para criar um item alquímico infundido que permite uma jogada de salvamento, você pode substituir a CD dele pela sua CD de classe. </t>
+  </si>
+  <si>
+    <t>BOMBA GRUDENTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequência uma vez por rodada Acionamento Você usa Alquimia Rápida para manufaturar uma bomba alquímica com nível de item pelo menos 2 níveis inferior ao seu nível de alquimia avançada. Você mistura um aditivo que faz o conteúdo de suas bombas aderir ao alvo e continuar a causar dano. Uma criatura que sofrer um acerto direto de uma de suas bombas grudentas também sofre dano persistente igual e do mesmo tipo que o dano de respingo da bomba. Se a bomba já causar dano persistente, some os dois valores. </t>
+  </si>
+  <si>
+    <t>MUTAGÊNICO FERAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seu mutagênico bestial traz à tona a sua besta interior, concedendo-lhe garras, dentes afiados e uma aparência feroz. Sempre que for afetado por um mutagênico bestial de sua criação, você recebe o bônus de item do mutagênico em seus testes de Intimidação. Além disso, suas garras e mandíbulas se tornam ainda mais ferozes, recebendo o traço mortal d10. Finalmente, você pode aumentar a penalidade do mutagênico na CA de –1 para –2 e, em troca, aumentar o tamanho do dado de dano de suas garras e mandíbulas em um passo. </t>
+  </si>
+  <si>
+    <t>BOMBA DEBILITANTE MAIOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré-requisitos Bomba Debilitante </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você aprendeu técnicas avançadas e segredos alquímicos para expandir as possibilidades de efeitos impostos por suas bombas. Quando usar Bomba Debilitante, adicione as seguintes opções à lista de efeitos que podem ser impostos: desajeitado 1, enfraquecido 1, estupefato 1, ou –3 metros de penalidade de estado em todas as Velocidades. </t>
+  </si>
+  <si>
+    <t>ELIXIR MISERICORDIOSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequência uma vez por rodada Acionamento Você usa Alquimia Rápida para manufaturar um elixir da vida com nível de item pelo menos 2 níveis inferior ao seu nível de alquimia avançada. Você mistura um aditivo especial em seu elixir que acalma o corpo e a mente de quem o ingere. O elixir da vida tenta neutralizar um efeito de medo ou que imponha a condição paralisado à criatura que o ingerir. </t>
+  </si>
+  <si>
+    <t>ENVENENADOR POTENTE</t>
+  </si>
+  <si>
+    <t>Pré-requisitos Alquimia Poderosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao concentrar os componentes tóxicos de seus venenos, você os torna mais difíceis de resistir. Quando manufaturar um item alquímico com o traço veneno através de qualquer meio, você aumenta a CD dele em até 4 pontos (até um máximo igual à sua CD de classe). </t>
+  </si>
+  <si>
+    <t>MUTAGÊNICO ELÁSTICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você faz seu corpo retorcer e fluir como o mercúrio dentro de seus mutagênicos. Sempre que estiver sob os efeitos de um mutagênico de mercúrio de sua criação, você pode esticar suas pernas e Dar um Passo de até 3 metros ou espremer e esmagar seu corpo, permitindo-lhe passar por espaços apertados como se fosse um tamanho menor (além dos efeitos de Espremer-se). </t>
+  </si>
+  <si>
+    <t>RESPINGO EXPANDIDO</t>
+  </si>
+  <si>
+    <t>Pré-requisitos Respingo Calculado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os componentes particularmente voláteis que você mistura em suas bombas resultam em explosões especialmente grandes e poderosas. Quando arremessar uma bomba alquímica de sua criação e essa bomba possuir o traço respingo, você pode adicionar seu modificador de Inteligência ao dano de respingo usual da bomba, e ela causa dano de respingo a todas as criaturas a até 3 metros do alvo. </t>
+  </si>
+  <si>
+    <t>BOMBAS EXCEPCIONAIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré-requisitos Lançador Longínquo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você lança bombas de maneira infalível, apesar de obstru- ções ou distância. Quando arremessar um item alquímico com o traço bomba, o incremento de distância dele aumenta para 18 metros, você também reduz quaisquer bônus de cir- cunstância à CA do alvo por cobertura em 1 ponto, e automa- ticamente obtém sucesso no teste simples para mirar uma criatura ocultada. </t>
+  </si>
+  <si>
+    <t>MUTAGÊNICO INVENCÍVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os aditivos fortificantes que você mistura em seus mutagênicos deixam a sua forma irrefreável ainda mais impenetrável. Sempre que for afetado por um mutagênico irrefreável de sua criação, você adquire resistência a todo dano físico igual ao seu valor de Inteligência (mínimo 0). </t>
+  </si>
+  <si>
+    <t>PROLONGAR ELIXIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao investir sua própria energia pessoal nos elixires que cria, você faz com que o afetem por mais tempo. Quando consumir um de seus itens alquímicos que possua os traços elixir e infundido e duração de 1 minuto ou mais, você dobra a duração desse elixir. </t>
+  </si>
+  <si>
+    <t>BOMBA DEBILITANTE VERDADEIRA</t>
+  </si>
+  <si>
+    <t>Pré-requisitos Bomba Debilitante Maior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sempre inventivo, você descobriu formas ainda mais devastadoras para impedir e refrear seus adversários com suas bombas. Quando usar Bomba Debilitante, adicione as seguintes opções à lista de efeitos que podem ser impostos: enfraquecido 2, estupefato 2, ou –4,5 metros de penalidade de estado em todas as Velocidades. Se você resolver aplicar um dos efeitos listados em Bomba Debilitante, o alvo evita o efeito apenas se o resultado da jogada de salvamento dele for um sucesso crítico. </t>
+  </si>
+  <si>
+    <t>ELIXIR MISERICORDIOSO MAIOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré-requisitos Elixir Misericordioso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seus aditivos contêm panaceias curativas capazes de remediar várias enfermidades. Quando você usar Elixir Misericordioso, seu elixir pode tentar neutralizar a condição cego, enjoado, lento ou surdo. </t>
+  </si>
+  <si>
+    <t>MUTAGÊNICO LOQUAZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seu mutagênico de língua de prata transcende idiomas e até a plausibilidade. Quando afetado por um mutagênico de língua de prata de sua criação, você ignora penalidades de circunstância em testes de Diplomacia, Dissimulação, Intimidação e Performance. Além disso, suas palavras transcendem as barreiras linguísticas; todos que lhe ouvirem falar compreendem suas palavras como se você estivesse falando o idioma deles (embora você não fale de fato esse idioma). Esta habilidade também não lhe permite compreender quaisquer idiomas adicionais. </t>
+  </si>
+  <si>
+    <t>BOMBA LANCINANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequência uma vez por rodada Acionamento Você usa Alquimia Rápida para manufaturar uma bomba alquímica com nível de item pelo menos 2 níveis inferior ao seu nível de alquimia avançada. Você mistura uma substância na bomba para reduzir as resistências de seu inimigo. A bomba reduz qualquer resistência que o inimigo possua ao tipo de dano da bomba em uma quantidade igual ao seu nível, mas apenas para esse ataque. </t>
+  </si>
+  <si>
+    <t>ELIXIR ETERNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré-requisitos Prolongar Elixir </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seu corpo prontamente aceita e retém mudanças menores. Quando consumir um de seus itens alquímicos que possua os traços elixir e infundido e duração de 1 minuto ou mais, a duração desse elixir é indefinida. Você só pode fazer isso se o nível do elixir for igual à metade de seu nível ou inferior. Se posteriormente consumir outro elixir e tornar sua duração indefinida, o efeito do elixir indefinido anterior é encerrado. </t>
+  </si>
+  <si>
+    <t>MUTAGÊNICO GENIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você realiza ajustes especializados na fórmula de seus mutagênicos cognitivos que amplificam sua genialidade para melhorar os benefícios recebidos. Sempre que for afetado por um mutagênico cognitivo de sua criação, você recebe o bônus de item do mutagênico em seus testes de Diplomacia, Dissimulação, Intimidação, Medicina, Natureza, Performance, Religião e Sobrevivência. Além disso, você pode comunicar-se telepaticamente com criaturas a até 18 metros caso compartilhem um idioma em comum. Depois de estabelecida, a comunicação passa a ser duas vias, fazendo com que uma criatura contatada também possa se comunicar com você. </t>
+  </si>
+  <si>
+    <t>MUTAGÊNICO PERSISTENTE</t>
+  </si>
+  <si>
+    <t>Você treinou sua forma física para em um determinado estado alterado. Uma vez por dia, quando consumir um item alquímico com os traços infundido e mutagênico de sua criação, você retém os efeitos dele até a próxima vez que fizer suas preparações diárias (em vez de considerar sua duração normal).</t>
+  </si>
+  <si>
+    <t>DEBILITAÇÃO PERFEITA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você aperfeiçoou as fórmulas de bombas que retardam seus inimigos. Quando usar Bomba Debilitante, seu alvo evita a condição imposta pela bomba apenas se obtiver um sucesso crítico em sua jogada de salvamento. </t>
+  </si>
+  <si>
+    <t>ELIXIRES IMPROVÁVEIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seu domínio de segredos alquímicos lhe permite replicar efeitos que alguns acreditam serem possíveis apenas através de magia. Selecione uma quantidade de poções igual ao seu modificador de Inteligência (mínimo 1) de 9o nível ou inferior. Você adquire fórmulas para Manufaturar estas poções como itens alquímicos com o traço elixir. Quando Manufaturar estes elixires alquímicos, você pode substituir reagentes alquímicos por um valor igual de componentes mágicos e usar ferramentas de alquimista em vez de quaisquer outros kits de ferramentas necessários. Exceto por isso, a fórmula não muda. Uma vez que tenha escolhido as fórmulas das poções, elas não podem ser alteradas. </t>
+  </si>
+  <si>
+    <t>MUTAGÊNICO DE MENTE LIMPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Com um ajuste mínimo nas proporções da fórmula de seu mutagênico sereno, você obtém proteções mentais. Quando for afetado por um mutagênico sereno de sua criação, efeitos de detecção, revelação e vidência de 9o nível ou inferior não detectam nada em você, suas posses e auras. Por exemplo, detectar magia ainda detectaria outras magias na área, mas não qualquer magia em você. </t>
+  </si>
+  <si>
+    <t>TRABALHADOR MILAGROSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequência uma vez a cada 10 minutos Seu domínio da alquimia pode ressuscitar os recentemente falecidos. Você pode administrar um elixir da vida verdadeiro a uma criatura que tenha morrido a 2 rodadas ou menos. Quando o fizer, essa criatura retorna imediatamente à vida com 1 Ponto de Vida e ferida 1. </t>
+  </si>
+  <si>
+    <t>CRIAR PEDRA FILOSOFAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sua longa pesquisa deu resultado, culminando na lendária pedra filosofal. Você aprende a fórmula para a pedra filosofal e pode acrescentá-la ao seu livro de fórmulas. </t>
+  </si>
+  <si>
+    <t>MEGA BOMBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré-requisitos Respingo Expandido </t>
+  </si>
+  <si>
+    <t>Requerimentos Você segura uma bomba alquímica infundida de sua criação e que tenha nível de item pelo menos 3 níveis inferiores ao seu nível de alquimia avançada. Você acrescenta um aditivo incrivelmente poderoso à bomba segurada para criar uma mega bomba, aumentando consideravelmente sua área e poder. Você usa uma ação de Interagir (em vez de Golpear) para arremessar a mega bomba e não realiza uma rolagem de ataque. A mega bomba afeta criaturas em uma explosão de 9 metros de raio, centrada a até 18 metros de você. A bomba causa dano como se cada criatura fosse o alvo primário, permitindo que realizem um salvamento básico de Reflexos. Se fracassar no salvamento, a criatura também sofre quaisquer efeitos que afetariam um alvo primário (como o efeito desprevenido de um relâmpago engarrafado). Embora todos os alvos na área sofram o dano de respingo como alvos primários, nenhum dano de respingo é causado a qualquer outra criatura além dessa área. Se a sua próxima ação após criar uma mega bomba não for uma ação de Interagir para arremessá-la, a mega bomba perde a potência e todos seus efeitos.</t>
+  </si>
+  <si>
+    <t>MUTAGÊNICO PERFEITO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Você aprimorou as fórmulas de seus mutagênicos, alinhando-os perfeitamente à sua fisiologia. Quando estiver sob os efeitos de um mutagênico de sua criação, você não sofre suas desvantagens. </t>
   </si>
 </sst>
 </file>
@@ -1004,8 +1269,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1288,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,4 +3881,629 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" t="s">
+        <v>326</v>
+      </c>
+      <c r="F5" t="s">
+        <v>317</v>
+      </c>
+      <c r="G5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>328</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>329</v>
+      </c>
+      <c r="F6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>331</v>
+      </c>
+      <c r="F7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>332</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>333</v>
+      </c>
+      <c r="F8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>334</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>335</v>
+      </c>
+      <c r="F9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>338</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" t="s">
+        <v>339</v>
+      </c>
+      <c r="F11" t="s">
+        <v>317</v>
+      </c>
+      <c r="G11" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>341</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>342</v>
+      </c>
+      <c r="F12" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>343</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" t="s">
+        <v>344</v>
+      </c>
+      <c r="F13" t="s">
+        <v>317</v>
+      </c>
+      <c r="G13" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>345</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>346</v>
+      </c>
+      <c r="F14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>347</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" t="s">
+        <v>348</v>
+      </c>
+      <c r="F15" t="s">
+        <v>317</v>
+      </c>
+      <c r="G15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>349</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>350</v>
+      </c>
+      <c r="F16" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>352</v>
+      </c>
+      <c r="E17" t="s">
+        <v>353</v>
+      </c>
+      <c r="F17" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>354</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" t="s">
+        <v>355</v>
+      </c>
+      <c r="F18" t="s">
+        <v>317</v>
+      </c>
+      <c r="G18" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>356</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>357</v>
+      </c>
+      <c r="E19" t="s">
+        <v>358</v>
+      </c>
+      <c r="F19" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>359</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>360</v>
+      </c>
+      <c r="F20" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>362</v>
+      </c>
+      <c r="E21" t="s">
+        <v>363</v>
+      </c>
+      <c r="F21" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>364</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>365</v>
+      </c>
+      <c r="E22" t="s">
+        <v>366</v>
+      </c>
+      <c r="F22" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>367</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>368</v>
+      </c>
+      <c r="F23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>369</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>370</v>
+      </c>
+      <c r="F24" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>371</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>372</v>
+      </c>
+      <c r="E25" t="s">
+        <v>373</v>
+      </c>
+      <c r="F25" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>374</v>
+      </c>
+      <c r="B26">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
+        <v>375</v>
+      </c>
+      <c r="E26" t="s">
+        <v>376</v>
+      </c>
+      <c r="F26" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>377</v>
+      </c>
+      <c r="B27">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>378</v>
+      </c>
+      <c r="F27" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>379</v>
+      </c>
+      <c r="B28">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>157</v>
+      </c>
+      <c r="E28" t="s">
+        <v>380</v>
+      </c>
+      <c r="F28" t="s">
+        <v>317</v>
+      </c>
+      <c r="G28" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>381</v>
+      </c>
+      <c r="B29">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>382</v>
+      </c>
+      <c r="E29" t="s">
+        <v>383</v>
+      </c>
+      <c r="F29" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>384</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>385</v>
+      </c>
+      <c r="F30" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>386</v>
+      </c>
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>382</v>
+      </c>
+      <c r="E31" t="s">
+        <v>387</v>
+      </c>
+      <c r="F31" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>388</v>
+      </c>
+      <c r="B32">
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>389</v>
+      </c>
+      <c r="F32" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>390</v>
+      </c>
+      <c r="B33">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>391</v>
+      </c>
+      <c r="F33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>392</v>
+      </c>
+      <c r="B34">
+        <v>18</v>
+      </c>
+      <c r="E34" t="s">
+        <v>393</v>
+      </c>
+      <c r="F34" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>394</v>
+      </c>
+      <c r="B35">
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>395</v>
+      </c>
+      <c r="F35" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>396</v>
+      </c>
+      <c r="B36">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>397</v>
+      </c>
+      <c r="F36" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>398</v>
+      </c>
+      <c r="B37">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" t="s">
+        <v>399</v>
+      </c>
+      <c r="E37" t="s">
+        <v>400</v>
+      </c>
+      <c r="F37" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>401</v>
+      </c>
+      <c r="B38">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>402</v>
+      </c>
+      <c r="F38" t="s">
+        <v>317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>